<commit_message>
Backup QR Scanner data - 2025-10-17T15:53:05.806Z - Cache Bust: 1760716385806
</commit_message>
<xml_diff>
--- a/log_history/Y3_B2526_Anatomy_scanner1760512521008_3549b8d920378e5cf953f077eab814bc6eeab41cbfa32d3c6e64714189cf06a0.xlsx
+++ b/log_history/Y3_B2526_Anatomy_scanner1760512521008_3549b8d920378e5cf953f077eab814bc6eeab41cbfa32d3c6e64714189cf06a0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Anatomy" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -862,9 +862,29 @@
         <v>hananragab@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>234035</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Anatomy</v>
+      </c>
+      <c r="C24" t="str">
+        <v>15/10/2025</v>
+      </c>
+      <c r="D24" t="str">
+        <v>12:54:40</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F24" t="str">
+        <v>hananragab@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>